<commit_message>
[Mod] Excel Data Add
</commit_message>
<xml_diff>
--- a/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
+++ b/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\HIGHFIVE\HIGHFIVE\Assets\Resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity_Project\TeamProject\Sparta06_TeamProject_HIGHFIVE\HIGHFIVE\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767B3CB7-CCDA-4E95-AA8C-058C8330F8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="31665" yWindow="2655" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>job</t>
   </si>
@@ -361,11 +362,15 @@
     <t>나무</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>sight</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -415,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -423,14 +428,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -714,11 +716,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -769,7 +771,9 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -805,7 +809,9 @@
       <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="1"/>
+      <c r="K2" s="1">
+        <v>3</v>
+      </c>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="16.5" customHeight="1">
@@ -839,7 +845,9 @@
       <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="1"/>
+      <c r="K3" s="1">
+        <v>3</v>
+      </c>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:14" ht="16.5" customHeight="1">
@@ -873,7 +881,9 @@
       <c r="J4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="1"/>
+      <c r="K4" s="1">
+        <v>3</v>
+      </c>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:14" ht="16.5" customHeight="1">
@@ -1883,7 +1893,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2983,10 +2993,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -2995,34 +3005,34 @@
     <col min="1" max="5" width="9.77734375" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="8" width="9.77734375" customWidth="1"/>
-    <col min="9" max="9" width="8.21875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="8.21875" style="3" customWidth="1"/>
     <col min="10" max="26" width="8.21875" customWidth="1"/>
     <col min="27" max="1025" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -3030,263 +3040,263 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>10</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>10</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>1</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>3</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>50</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>50</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>10</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>10</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>1</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>3</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>3</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>50</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>50</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>10</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>10</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>3</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>3</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>50</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>50</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>10</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>10</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>1</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>3</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>3</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>50</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>50</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>10</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>10</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>1</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>3</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>3</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>50</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>50</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>10</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>10</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>3</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>3</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>50</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>50</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>10</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>10</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>3</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>3</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>50</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>50</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>10</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>10</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>3</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>3</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>50</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>50</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="3">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>10</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>10</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>3</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>3</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>50</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>50</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="3">
         <v>30</v>
       </c>
     </row>
@@ -4288,7 +4298,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -4307,176 +4317,176 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>100</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>20</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>0</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>0</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>100</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>5</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>30</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>0</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>100</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>0</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>0</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>5</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>100</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>0</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>0</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>20</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>100</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>0</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>0</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>0</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Mod] StateMachine Idle, Move FIx / InputAction Fix / Refactoring
</commit_message>
<xml_diff>
--- a/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
+++ b/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\HIGHFIVE\HIGHFIVE\Assets\Resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity_Project\TeamProject\Sparta06_TeamProject_HIGHFIVE\HIGHFIVE\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F55E4D-C67B-4131-A1EF-A1F312E3E847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="31665" yWindow="2655" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -200,12 +201,6 @@
     <t>나무</t>
   </si>
   <si>
-    <t>NM2</t>
-  </si>
-  <si>
-    <t>NM3</t>
-  </si>
-  <si>
     <t>EL1</t>
   </si>
   <si>
@@ -367,11 +362,19 @@
     <t>sight</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>NM3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NM2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -422,7 +425,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -431,7 +434,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -713,7 +716,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
@@ -1890,7 +1893,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2990,11 +2993,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3036,7 +3039,7 @@
         <v>26</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1">
@@ -3068,12 +3071,12 @@
         <v>3</v>
       </c>
       <c r="J2" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B3" s="5">
         <v>10</v>
@@ -3105,7 +3108,7 @@
     </row>
     <row r="4" spans="1:10" ht="16.5" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B4" s="5">
         <v>10</v>
@@ -3137,7 +3140,7 @@
     </row>
     <row r="5" spans="1:10" ht="16.5" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="5">
         <v>10</v>
@@ -3169,7 +3172,7 @@
     </row>
     <row r="6" spans="1:10" ht="16.5" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="5">
         <v>10</v>
@@ -3201,7 +3204,7 @@
     </row>
     <row r="7" spans="1:10" ht="16.5" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="5">
         <v>10</v>
@@ -3233,7 +3236,7 @@
     </row>
     <row r="8" spans="1:10" ht="16.5" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" s="5">
         <v>10</v>
@@ -3265,7 +3268,7 @@
     </row>
     <row r="9" spans="1:10" ht="16.5" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" s="5">
         <v>10</v>
@@ -3297,7 +3300,7 @@
     </row>
     <row r="10" spans="1:10" ht="16.5" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5">
         <v>10</v>
@@ -4325,10 +4328,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -4345,31 +4350,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1">
@@ -4377,13 +4382,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="E2" s="5">
         <v>100</v>
@@ -4406,13 +4411,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E3" s="5">
         <v>100</v>
@@ -4435,13 +4440,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" s="5">
         <v>100</v>
@@ -4464,13 +4469,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E5" s="5">
         <v>100</v>
@@ -4493,13 +4498,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6" s="5">
         <v>100</v>

</xml_diff>

<commit_message>
[Mod] Excel 수치 조정
</commit_message>
<xml_diff>
--- a/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
+++ b/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity_Project\TeamProject\Sparta06_TeamProject_HIGHFIVE\HIGHFIVE\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C03EAB5-7170-4D7C-B4AC-7632B021FE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE685D1A-E75C-49B2-9D62-61AA6D048E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31665" yWindow="2655" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6840" yWindow="1650" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -719,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -2996,8 +2996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3050,13 +3050,13 @@
         <v>10</v>
       </c>
       <c r="C2" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
       </c>
       <c r="E2" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" s="5">
         <v>3</v>
@@ -3068,7 +3068,7 @@
         <v>50</v>
       </c>
       <c r="I2" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J2" s="5">
         <v>4</v>
@@ -3082,13 +3082,13 @@
         <v>10</v>
       </c>
       <c r="C3" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
       </c>
       <c r="E3" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" s="5">
         <v>3</v>
@@ -3114,13 +3114,13 @@
         <v>10</v>
       </c>
       <c r="C4" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
       </c>
       <c r="E4" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" s="5">
         <v>3</v>
@@ -3146,13 +3146,13 @@
         <v>10</v>
       </c>
       <c r="C5" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="E5" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" s="5">
         <v>3</v>
@@ -3178,13 +3178,13 @@
         <v>10</v>
       </c>
       <c r="C6" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
       </c>
       <c r="E6" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="5">
         <v>3</v>
@@ -3210,13 +3210,13 @@
         <v>10</v>
       </c>
       <c r="C7" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D7" s="5">
         <v>1</v>
       </c>
       <c r="E7" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" s="5">
         <v>3</v>
@@ -3242,13 +3242,13 @@
         <v>10</v>
       </c>
       <c r="C8" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
       </c>
       <c r="E8" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" s="5">
         <v>3</v>
@@ -3274,13 +3274,13 @@
         <v>10</v>
       </c>
       <c r="C9" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D9" s="5">
         <v>1</v>
       </c>
       <c r="E9" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" s="5">
         <v>3</v>
@@ -3306,13 +3306,13 @@
         <v>10</v>
       </c>
       <c r="C10" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D10" s="5">
         <v>1</v>
       </c>
       <c r="E10" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" s="5">
         <v>3</v>

</xml_diff>

<commit_message>
[Fix] All Scene UI Fix
UI에셋 수정
</commit_message>
<xml_diff>
--- a/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
+++ b/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity_Project\TeamProject\Sparta06_TeamProject_HIGHFIVE\HIGHFIVE\Assets\Resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\HIGHFIVE\HIGHFIVE\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE685D1A-E75C-49B2-9D62-61AA6D048E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="1650" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6840" yWindow="1650" windowWidth="21600" windowHeight="11385" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
     <sheet name="Skills" sheetId="2" r:id="rId2"/>
     <sheet name="Monsters" sheetId="3" r:id="rId3"/>
     <sheet name="Items" sheetId="4" r:id="rId4"/>
+    <sheet name="BUFF" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="80">
   <si>
     <t>job</t>
   </si>
@@ -201,15 +201,6 @@
     <t>나무</t>
   </si>
   <si>
-    <t>EL1</t>
-  </si>
-  <si>
-    <t>EL2</t>
-  </si>
-  <si>
-    <t>EL3</t>
-  </si>
-  <si>
     <t>EL4</t>
   </si>
   <si>
@@ -363,18 +354,142 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>NM3</t>
+    <t>설명</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>NM2</t>
+    <t>오거</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>오거 전사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>에픽</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>블루</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>레드</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마법사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마법사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>도적</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>도적</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>도적</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상승치</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>스텟</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>패자의 분노</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>레드</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>블루</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>배틀 페이즈에서 패배했을 시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>조건</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>레드 몬스터 처치 시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>블루 몬스터 처치 시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>에픽</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>에픽 몬스터 처치 시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파이어볼</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>번개</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>매직미사일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>헤이스트</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>일섬</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>은신</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -716,10 +831,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -1893,18 +2008,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9.77734375" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="6" width="9.77734375" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" customWidth="1"/>
+    <col min="4" max="6" width="9.77734375" customWidth="1"/>
     <col min="7" max="26" width="8.21875" customWidth="1"/>
     <col min="27" max="1025" width="12" customWidth="1"/>
   </cols>
@@ -1959,41 +2075,95 @@
         <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="D4" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="16.5" customHeight="1"/>
     <row r="12" spans="1:4" ht="16.5" customHeight="1"/>
@@ -2993,11 +3163,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3039,7 +3209,7 @@
         <v>26</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1">
@@ -3071,18 +3241,18 @@
         <v>10</v>
       </c>
       <c r="J2" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B3" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
@@ -3100,7 +3270,7 @@
         <v>50</v>
       </c>
       <c r="I3" s="3">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="J3" s="5">
         <v>3</v>
@@ -3108,13 +3278,13 @@
     </row>
     <row r="4" spans="1:10" ht="16.5" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="5">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
@@ -3123,16 +3293,16 @@
         <v>2</v>
       </c>
       <c r="F4" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4" s="5">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H4" s="5">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="I4" s="3">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="J4" s="5">
         <v>3</v>
@@ -3140,13 +3310,13 @@
     </row>
     <row r="5" spans="1:10" ht="16.5" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B5" s="5">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
@@ -3158,27 +3328,27 @@
         <v>3</v>
       </c>
       <c r="G5" s="5">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="H5" s="5">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="I5" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J5" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="16.5" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="B6" s="5">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C6" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
@@ -3190,30 +3360,30 @@
         <v>3</v>
       </c>
       <c r="G6" s="5">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="H6" s="5">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="I6" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J6" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.5" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B7" s="5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D7" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="5">
         <v>2</v>
@@ -3222,21 +3392,21 @@
         <v>3</v>
       </c>
       <c r="G7" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H7" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I7" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="J7" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="16.5" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" s="5">
         <v>10</v>
@@ -3268,7 +3438,7 @@
     </row>
     <row r="9" spans="1:10" ht="16.5" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B9" s="5">
         <v>10</v>
@@ -3300,7 +3470,7 @@
     </row>
     <row r="10" spans="1:10" ht="16.5" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5">
         <v>10</v>
@@ -4328,7 +4498,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4350,31 +4520,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1">
@@ -4382,13 +4552,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E2" s="5">
         <v>100</v>
@@ -4411,13 +4581,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E3" s="5">
         <v>100</v>
@@ -4440,13 +4610,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E4" s="5">
         <v>100</v>
@@ -4469,13 +4639,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E5" s="5">
         <v>100</v>
@@ -4498,13 +4668,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E6" s="5">
         <v>100</v>
@@ -5521,4 +5691,1132 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1000"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" customWidth="1"/>
+    <col min="2" max="2" width="35.21875" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="5" max="6" width="9.77734375" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" customWidth="1"/>
+    <col min="8" max="9" width="9.77734375" customWidth="1"/>
+    <col min="10" max="26" width="8.21875" customWidth="1"/>
+    <col min="27" max="1025" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16.5" customHeight="1">
+      <c r="A1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" ht="16.5" customHeight="1">
+      <c r="A2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="16.5" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="5">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" ht="16.5" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" ht="16.5" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="16.5" customHeight="1">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="16.5" customHeight="1"/>
+    <row r="8" spans="1:9" ht="16.5" customHeight="1"/>
+    <row r="9" spans="1:9" ht="16.5" customHeight="1"/>
+    <row r="10" spans="1:9" ht="16.5" customHeight="1"/>
+    <row r="11" spans="1:9" ht="16.5" customHeight="1"/>
+    <row r="12" spans="1:9" ht="16.5" customHeight="1"/>
+    <row r="13" spans="1:9" ht="16.5" customHeight="1"/>
+    <row r="14" spans="1:9" ht="16.5" customHeight="1"/>
+    <row r="15" spans="1:9" ht="16.5" customHeight="1"/>
+    <row r="16" spans="1:9" ht="16.5" customHeight="1"/>
+    <row r="17" ht="16.5" customHeight="1"/>
+    <row r="18" ht="16.5" customHeight="1"/>
+    <row r="19" ht="16.5" customHeight="1"/>
+    <row r="20" ht="16.5" customHeight="1"/>
+    <row r="21" ht="16.5" customHeight="1"/>
+    <row r="22" ht="16.5" customHeight="1"/>
+    <row r="23" ht="16.5" customHeight="1"/>
+    <row r="24" ht="16.5" customHeight="1"/>
+    <row r="25" ht="16.5" customHeight="1"/>
+    <row r="26" ht="16.5" customHeight="1"/>
+    <row r="27" ht="16.5" customHeight="1"/>
+    <row r="28" ht="16.5" customHeight="1"/>
+    <row r="29" ht="16.5" customHeight="1"/>
+    <row r="30" ht="16.5" customHeight="1"/>
+    <row r="31" ht="16.5" customHeight="1"/>
+    <row r="32" ht="16.5" customHeight="1"/>
+    <row r="33" ht="16.5" customHeight="1"/>
+    <row r="34" ht="16.5" customHeight="1"/>
+    <row r="35" ht="16.5" customHeight="1"/>
+    <row r="36" ht="16.5" customHeight="1"/>
+    <row r="37" ht="16.5" customHeight="1"/>
+    <row r="38" ht="16.5" customHeight="1"/>
+    <row r="39" ht="16.5" customHeight="1"/>
+    <row r="40" ht="16.5" customHeight="1"/>
+    <row r="41" ht="16.5" customHeight="1"/>
+    <row r="42" ht="16.5" customHeight="1"/>
+    <row r="43" ht="16.5" customHeight="1"/>
+    <row r="44" ht="16.5" customHeight="1"/>
+    <row r="45" ht="16.5" customHeight="1"/>
+    <row r="46" ht="16.5" customHeight="1"/>
+    <row r="47" ht="16.5" customHeight="1"/>
+    <row r="48" ht="16.5" customHeight="1"/>
+    <row r="49" ht="16.5" customHeight="1"/>
+    <row r="50" ht="16.5" customHeight="1"/>
+    <row r="51" ht="16.5" customHeight="1"/>
+    <row r="52" ht="16.5" customHeight="1"/>
+    <row r="53" ht="16.5" customHeight="1"/>
+    <row r="54" ht="16.5" customHeight="1"/>
+    <row r="55" ht="16.5" customHeight="1"/>
+    <row r="56" ht="16.5" customHeight="1"/>
+    <row r="57" ht="16.5" customHeight="1"/>
+    <row r="58" ht="16.5" customHeight="1"/>
+    <row r="59" ht="16.5" customHeight="1"/>
+    <row r="60" ht="16.5" customHeight="1"/>
+    <row r="61" ht="16.5" customHeight="1"/>
+    <row r="62" ht="16.5" customHeight="1"/>
+    <row r="63" ht="16.5" customHeight="1"/>
+    <row r="64" ht="16.5" customHeight="1"/>
+    <row r="65" ht="16.5" customHeight="1"/>
+    <row r="66" ht="16.5" customHeight="1"/>
+    <row r="67" ht="16.5" customHeight="1"/>
+    <row r="68" ht="16.5" customHeight="1"/>
+    <row r="69" ht="16.5" customHeight="1"/>
+    <row r="70" ht="16.5" customHeight="1"/>
+    <row r="71" ht="16.5" customHeight="1"/>
+    <row r="72" ht="16.5" customHeight="1"/>
+    <row r="73" ht="16.5" customHeight="1"/>
+    <row r="74" ht="16.5" customHeight="1"/>
+    <row r="75" ht="16.5" customHeight="1"/>
+    <row r="76" ht="16.5" customHeight="1"/>
+    <row r="77" ht="16.5" customHeight="1"/>
+    <row r="78" ht="16.5" customHeight="1"/>
+    <row r="79" ht="16.5" customHeight="1"/>
+    <row r="80" ht="16.5" customHeight="1"/>
+    <row r="81" ht="16.5" customHeight="1"/>
+    <row r="82" ht="16.5" customHeight="1"/>
+    <row r="83" ht="16.5" customHeight="1"/>
+    <row r="84" ht="16.5" customHeight="1"/>
+    <row r="85" ht="16.5" customHeight="1"/>
+    <row r="86" ht="16.5" customHeight="1"/>
+    <row r="87" ht="16.5" customHeight="1"/>
+    <row r="88" ht="16.5" customHeight="1"/>
+    <row r="89" ht="16.5" customHeight="1"/>
+    <row r="90" ht="16.5" customHeight="1"/>
+    <row r="91" ht="16.5" customHeight="1"/>
+    <row r="92" ht="16.5" customHeight="1"/>
+    <row r="93" ht="16.5" customHeight="1"/>
+    <row r="94" ht="16.5" customHeight="1"/>
+    <row r="95" ht="16.5" customHeight="1"/>
+    <row r="96" ht="16.5" customHeight="1"/>
+    <row r="97" ht="16.5" customHeight="1"/>
+    <row r="98" ht="16.5" customHeight="1"/>
+    <row r="99" ht="16.5" customHeight="1"/>
+    <row r="100" ht="16.5" customHeight="1"/>
+    <row r="101" ht="16.5" customHeight="1"/>
+    <row r="102" ht="16.5" customHeight="1"/>
+    <row r="103" ht="16.5" customHeight="1"/>
+    <row r="104" ht="16.5" customHeight="1"/>
+    <row r="105" ht="16.5" customHeight="1"/>
+    <row r="106" ht="16.5" customHeight="1"/>
+    <row r="107" ht="16.5" customHeight="1"/>
+    <row r="108" ht="16.5" customHeight="1"/>
+    <row r="109" ht="16.5" customHeight="1"/>
+    <row r="110" ht="16.5" customHeight="1"/>
+    <row r="111" ht="16.5" customHeight="1"/>
+    <row r="112" ht="16.5" customHeight="1"/>
+    <row r="113" ht="16.5" customHeight="1"/>
+    <row r="114" ht="16.5" customHeight="1"/>
+    <row r="115" ht="16.5" customHeight="1"/>
+    <row r="116" ht="16.5" customHeight="1"/>
+    <row r="117" ht="16.5" customHeight="1"/>
+    <row r="118" ht="16.5" customHeight="1"/>
+    <row r="119" ht="16.5" customHeight="1"/>
+    <row r="120" ht="16.5" customHeight="1"/>
+    <row r="121" ht="16.5" customHeight="1"/>
+    <row r="122" ht="16.5" customHeight="1"/>
+    <row r="123" ht="16.5" customHeight="1"/>
+    <row r="124" ht="16.5" customHeight="1"/>
+    <row r="125" ht="16.5" customHeight="1"/>
+    <row r="126" ht="16.5" customHeight="1"/>
+    <row r="127" ht="16.5" customHeight="1"/>
+    <row r="128" ht="16.5" customHeight="1"/>
+    <row r="129" ht="16.5" customHeight="1"/>
+    <row r="130" ht="16.5" customHeight="1"/>
+    <row r="131" ht="16.5" customHeight="1"/>
+    <row r="132" ht="16.5" customHeight="1"/>
+    <row r="133" ht="16.5" customHeight="1"/>
+    <row r="134" ht="16.5" customHeight="1"/>
+    <row r="135" ht="16.5" customHeight="1"/>
+    <row r="136" ht="16.5" customHeight="1"/>
+    <row r="137" ht="16.5" customHeight="1"/>
+    <row r="138" ht="16.5" customHeight="1"/>
+    <row r="139" ht="16.5" customHeight="1"/>
+    <row r="140" ht="16.5" customHeight="1"/>
+    <row r="141" ht="16.5" customHeight="1"/>
+    <row r="142" ht="16.5" customHeight="1"/>
+    <row r="143" ht="16.5" customHeight="1"/>
+    <row r="144" ht="16.5" customHeight="1"/>
+    <row r="145" ht="16.5" customHeight="1"/>
+    <row r="146" ht="16.5" customHeight="1"/>
+    <row r="147" ht="16.5" customHeight="1"/>
+    <row r="148" ht="16.5" customHeight="1"/>
+    <row r="149" ht="16.5" customHeight="1"/>
+    <row r="150" ht="16.5" customHeight="1"/>
+    <row r="151" ht="16.5" customHeight="1"/>
+    <row r="152" ht="16.5" customHeight="1"/>
+    <row r="153" ht="16.5" customHeight="1"/>
+    <row r="154" ht="16.5" customHeight="1"/>
+    <row r="155" ht="16.5" customHeight="1"/>
+    <row r="156" ht="16.5" customHeight="1"/>
+    <row r="157" ht="16.5" customHeight="1"/>
+    <row r="158" ht="16.5" customHeight="1"/>
+    <row r="159" ht="16.5" customHeight="1"/>
+    <row r="160" ht="16.5" customHeight="1"/>
+    <row r="161" ht="16.5" customHeight="1"/>
+    <row r="162" ht="16.5" customHeight="1"/>
+    <row r="163" ht="16.5" customHeight="1"/>
+    <row r="164" ht="16.5" customHeight="1"/>
+    <row r="165" ht="16.5" customHeight="1"/>
+    <row r="166" ht="16.5" customHeight="1"/>
+    <row r="167" ht="16.5" customHeight="1"/>
+    <row r="168" ht="16.5" customHeight="1"/>
+    <row r="169" ht="16.5" customHeight="1"/>
+    <row r="170" ht="16.5" customHeight="1"/>
+    <row r="171" ht="16.5" customHeight="1"/>
+    <row r="172" ht="16.5" customHeight="1"/>
+    <row r="173" ht="16.5" customHeight="1"/>
+    <row r="174" ht="16.5" customHeight="1"/>
+    <row r="175" ht="16.5" customHeight="1"/>
+    <row r="176" ht="16.5" customHeight="1"/>
+    <row r="177" ht="16.5" customHeight="1"/>
+    <row r="178" ht="16.5" customHeight="1"/>
+    <row r="179" ht="16.5" customHeight="1"/>
+    <row r="180" ht="16.5" customHeight="1"/>
+    <row r="181" ht="16.5" customHeight="1"/>
+    <row r="182" ht="16.5" customHeight="1"/>
+    <row r="183" ht="16.5" customHeight="1"/>
+    <row r="184" ht="16.5" customHeight="1"/>
+    <row r="185" ht="16.5" customHeight="1"/>
+    <row r="186" ht="16.5" customHeight="1"/>
+    <row r="187" ht="16.5" customHeight="1"/>
+    <row r="188" ht="16.5" customHeight="1"/>
+    <row r="189" ht="16.5" customHeight="1"/>
+    <row r="190" ht="16.5" customHeight="1"/>
+    <row r="191" ht="16.5" customHeight="1"/>
+    <row r="192" ht="16.5" customHeight="1"/>
+    <row r="193" ht="16.5" customHeight="1"/>
+    <row r="194" ht="16.5" customHeight="1"/>
+    <row r="195" ht="16.5" customHeight="1"/>
+    <row r="196" ht="16.5" customHeight="1"/>
+    <row r="197" ht="16.5" customHeight="1"/>
+    <row r="198" ht="16.5" customHeight="1"/>
+    <row r="199" ht="16.5" customHeight="1"/>
+    <row r="200" ht="16.5" customHeight="1"/>
+    <row r="201" ht="16.5" customHeight="1"/>
+    <row r="202" ht="16.5" customHeight="1"/>
+    <row r="203" ht="16.5" customHeight="1"/>
+    <row r="204" ht="16.5" customHeight="1"/>
+    <row r="205" ht="16.5" customHeight="1"/>
+    <row r="206" ht="16.5" customHeight="1"/>
+    <row r="207" ht="16.5" customHeight="1"/>
+    <row r="208" ht="16.5" customHeight="1"/>
+    <row r="209" ht="16.5" customHeight="1"/>
+    <row r="210" ht="16.5" customHeight="1"/>
+    <row r="211" ht="16.5" customHeight="1"/>
+    <row r="212" ht="16.5" customHeight="1"/>
+    <row r="213" ht="16.5" customHeight="1"/>
+    <row r="214" ht="16.5" customHeight="1"/>
+    <row r="215" ht="16.5" customHeight="1"/>
+    <row r="216" ht="16.5" customHeight="1"/>
+    <row r="217" ht="16.5" customHeight="1"/>
+    <row r="218" ht="16.5" customHeight="1"/>
+    <row r="219" ht="16.5" customHeight="1"/>
+    <row r="220" ht="16.5" customHeight="1"/>
+    <row r="221" ht="16.5" customHeight="1"/>
+    <row r="222" ht="16.5" customHeight="1"/>
+    <row r="223" ht="16.5" customHeight="1"/>
+    <row r="224" ht="16.5" customHeight="1"/>
+    <row r="225" ht="16.5" customHeight="1"/>
+    <row r="226" ht="16.5" customHeight="1"/>
+    <row r="227" ht="16.5" customHeight="1"/>
+    <row r="228" ht="16.5" customHeight="1"/>
+    <row r="229" ht="16.5" customHeight="1"/>
+    <row r="230" ht="16.5" customHeight="1"/>
+    <row r="231" ht="16.5" customHeight="1"/>
+    <row r="232" ht="16.5" customHeight="1"/>
+    <row r="233" ht="16.5" customHeight="1"/>
+    <row r="234" ht="16.5" customHeight="1"/>
+    <row r="235" ht="16.5" customHeight="1"/>
+    <row r="236" ht="16.5" customHeight="1"/>
+    <row r="237" ht="16.5" customHeight="1"/>
+    <row r="238" ht="16.5" customHeight="1"/>
+    <row r="239" ht="16.5" customHeight="1"/>
+    <row r="240" ht="16.5" customHeight="1"/>
+    <row r="241" ht="16.5" customHeight="1"/>
+    <row r="242" ht="16.5" customHeight="1"/>
+    <row r="243" ht="16.5" customHeight="1"/>
+    <row r="244" ht="16.5" customHeight="1"/>
+    <row r="245" ht="16.5" customHeight="1"/>
+    <row r="246" ht="16.5" customHeight="1"/>
+    <row r="247" ht="16.5" customHeight="1"/>
+    <row r="248" ht="16.5" customHeight="1"/>
+    <row r="249" ht="16.5" customHeight="1"/>
+    <row r="250" ht="16.5" customHeight="1"/>
+    <row r="251" ht="16.5" customHeight="1"/>
+    <row r="252" ht="16.5" customHeight="1"/>
+    <row r="253" ht="16.5" customHeight="1"/>
+    <row r="254" ht="16.5" customHeight="1"/>
+    <row r="255" ht="16.5" customHeight="1"/>
+    <row r="256" ht="16.5" customHeight="1"/>
+    <row r="257" ht="16.5" customHeight="1"/>
+    <row r="258" ht="16.5" customHeight="1"/>
+    <row r="259" ht="16.5" customHeight="1"/>
+    <row r="260" ht="16.5" customHeight="1"/>
+    <row r="261" ht="16.5" customHeight="1"/>
+    <row r="262" ht="16.5" customHeight="1"/>
+    <row r="263" ht="16.5" customHeight="1"/>
+    <row r="264" ht="16.5" customHeight="1"/>
+    <row r="265" ht="16.5" customHeight="1"/>
+    <row r="266" ht="16.5" customHeight="1"/>
+    <row r="267" ht="16.5" customHeight="1"/>
+    <row r="268" ht="16.5" customHeight="1"/>
+    <row r="269" ht="16.5" customHeight="1"/>
+    <row r="270" ht="16.5" customHeight="1"/>
+    <row r="271" ht="16.5" customHeight="1"/>
+    <row r="272" ht="16.5" customHeight="1"/>
+    <row r="273" ht="16.5" customHeight="1"/>
+    <row r="274" ht="16.5" customHeight="1"/>
+    <row r="275" ht="16.5" customHeight="1"/>
+    <row r="276" ht="16.5" customHeight="1"/>
+    <row r="277" ht="16.5" customHeight="1"/>
+    <row r="278" ht="16.5" customHeight="1"/>
+    <row r="279" ht="16.5" customHeight="1"/>
+    <row r="280" ht="16.5" customHeight="1"/>
+    <row r="281" ht="16.5" customHeight="1"/>
+    <row r="282" ht="16.5" customHeight="1"/>
+    <row r="283" ht="16.5" customHeight="1"/>
+    <row r="284" ht="16.5" customHeight="1"/>
+    <row r="285" ht="16.5" customHeight="1"/>
+    <row r="286" ht="16.5" customHeight="1"/>
+    <row r="287" ht="16.5" customHeight="1"/>
+    <row r="288" ht="16.5" customHeight="1"/>
+    <row r="289" ht="16.5" customHeight="1"/>
+    <row r="290" ht="16.5" customHeight="1"/>
+    <row r="291" ht="16.5" customHeight="1"/>
+    <row r="292" ht="16.5" customHeight="1"/>
+    <row r="293" ht="16.5" customHeight="1"/>
+    <row r="294" ht="16.5" customHeight="1"/>
+    <row r="295" ht="16.5" customHeight="1"/>
+    <row r="296" ht="16.5" customHeight="1"/>
+    <row r="297" ht="16.5" customHeight="1"/>
+    <row r="298" ht="16.5" customHeight="1"/>
+    <row r="299" ht="16.5" customHeight="1"/>
+    <row r="300" ht="16.5" customHeight="1"/>
+    <row r="301" ht="16.5" customHeight="1"/>
+    <row r="302" ht="16.5" customHeight="1"/>
+    <row r="303" ht="16.5" customHeight="1"/>
+    <row r="304" ht="16.5" customHeight="1"/>
+    <row r="305" ht="16.5" customHeight="1"/>
+    <row r="306" ht="16.5" customHeight="1"/>
+    <row r="307" ht="16.5" customHeight="1"/>
+    <row r="308" ht="16.5" customHeight="1"/>
+    <row r="309" ht="16.5" customHeight="1"/>
+    <row r="310" ht="16.5" customHeight="1"/>
+    <row r="311" ht="16.5" customHeight="1"/>
+    <row r="312" ht="16.5" customHeight="1"/>
+    <row r="313" ht="16.5" customHeight="1"/>
+    <row r="314" ht="16.5" customHeight="1"/>
+    <row r="315" ht="16.5" customHeight="1"/>
+    <row r="316" ht="16.5" customHeight="1"/>
+    <row r="317" ht="16.5" customHeight="1"/>
+    <row r="318" ht="16.5" customHeight="1"/>
+    <row r="319" ht="16.5" customHeight="1"/>
+    <row r="320" ht="16.5" customHeight="1"/>
+    <row r="321" ht="16.5" customHeight="1"/>
+    <row r="322" ht="16.5" customHeight="1"/>
+    <row r="323" ht="16.5" customHeight="1"/>
+    <row r="324" ht="16.5" customHeight="1"/>
+    <row r="325" ht="16.5" customHeight="1"/>
+    <row r="326" ht="16.5" customHeight="1"/>
+    <row r="327" ht="16.5" customHeight="1"/>
+    <row r="328" ht="16.5" customHeight="1"/>
+    <row r="329" ht="16.5" customHeight="1"/>
+    <row r="330" ht="16.5" customHeight="1"/>
+    <row r="331" ht="16.5" customHeight="1"/>
+    <row r="332" ht="16.5" customHeight="1"/>
+    <row r="333" ht="16.5" customHeight="1"/>
+    <row r="334" ht="16.5" customHeight="1"/>
+    <row r="335" ht="16.5" customHeight="1"/>
+    <row r="336" ht="16.5" customHeight="1"/>
+    <row r="337" ht="16.5" customHeight="1"/>
+    <row r="338" ht="16.5" customHeight="1"/>
+    <row r="339" ht="16.5" customHeight="1"/>
+    <row r="340" ht="16.5" customHeight="1"/>
+    <row r="341" ht="16.5" customHeight="1"/>
+    <row r="342" ht="16.5" customHeight="1"/>
+    <row r="343" ht="16.5" customHeight="1"/>
+    <row r="344" ht="16.5" customHeight="1"/>
+    <row r="345" ht="16.5" customHeight="1"/>
+    <row r="346" ht="16.5" customHeight="1"/>
+    <row r="347" ht="16.5" customHeight="1"/>
+    <row r="348" ht="16.5" customHeight="1"/>
+    <row r="349" ht="16.5" customHeight="1"/>
+    <row r="350" ht="16.5" customHeight="1"/>
+    <row r="351" ht="16.5" customHeight="1"/>
+    <row r="352" ht="16.5" customHeight="1"/>
+    <row r="353" ht="16.5" customHeight="1"/>
+    <row r="354" ht="16.5" customHeight="1"/>
+    <row r="355" ht="16.5" customHeight="1"/>
+    <row r="356" ht="16.5" customHeight="1"/>
+    <row r="357" ht="16.5" customHeight="1"/>
+    <row r="358" ht="16.5" customHeight="1"/>
+    <row r="359" ht="16.5" customHeight="1"/>
+    <row r="360" ht="16.5" customHeight="1"/>
+    <row r="361" ht="16.5" customHeight="1"/>
+    <row r="362" ht="16.5" customHeight="1"/>
+    <row r="363" ht="16.5" customHeight="1"/>
+    <row r="364" ht="16.5" customHeight="1"/>
+    <row r="365" ht="16.5" customHeight="1"/>
+    <row r="366" ht="16.5" customHeight="1"/>
+    <row r="367" ht="16.5" customHeight="1"/>
+    <row r="368" ht="16.5" customHeight="1"/>
+    <row r="369" ht="16.5" customHeight="1"/>
+    <row r="370" ht="16.5" customHeight="1"/>
+    <row r="371" ht="16.5" customHeight="1"/>
+    <row r="372" ht="16.5" customHeight="1"/>
+    <row r="373" ht="16.5" customHeight="1"/>
+    <row r="374" ht="16.5" customHeight="1"/>
+    <row r="375" ht="16.5" customHeight="1"/>
+    <row r="376" ht="16.5" customHeight="1"/>
+    <row r="377" ht="16.5" customHeight="1"/>
+    <row r="378" ht="16.5" customHeight="1"/>
+    <row r="379" ht="16.5" customHeight="1"/>
+    <row r="380" ht="16.5" customHeight="1"/>
+    <row r="381" ht="16.5" customHeight="1"/>
+    <row r="382" ht="16.5" customHeight="1"/>
+    <row r="383" ht="16.5" customHeight="1"/>
+    <row r="384" ht="16.5" customHeight="1"/>
+    <row r="385" ht="16.5" customHeight="1"/>
+    <row r="386" ht="16.5" customHeight="1"/>
+    <row r="387" ht="16.5" customHeight="1"/>
+    <row r="388" ht="16.5" customHeight="1"/>
+    <row r="389" ht="16.5" customHeight="1"/>
+    <row r="390" ht="16.5" customHeight="1"/>
+    <row r="391" ht="16.5" customHeight="1"/>
+    <row r="392" ht="16.5" customHeight="1"/>
+    <row r="393" ht="16.5" customHeight="1"/>
+    <row r="394" ht="16.5" customHeight="1"/>
+    <row r="395" ht="16.5" customHeight="1"/>
+    <row r="396" ht="16.5" customHeight="1"/>
+    <row r="397" ht="16.5" customHeight="1"/>
+    <row r="398" ht="16.5" customHeight="1"/>
+    <row r="399" ht="16.5" customHeight="1"/>
+    <row r="400" ht="16.5" customHeight="1"/>
+    <row r="401" ht="16.5" customHeight="1"/>
+    <row r="402" ht="16.5" customHeight="1"/>
+    <row r="403" ht="16.5" customHeight="1"/>
+    <row r="404" ht="16.5" customHeight="1"/>
+    <row r="405" ht="16.5" customHeight="1"/>
+    <row r="406" ht="16.5" customHeight="1"/>
+    <row r="407" ht="16.5" customHeight="1"/>
+    <row r="408" ht="16.5" customHeight="1"/>
+    <row r="409" ht="16.5" customHeight="1"/>
+    <row r="410" ht="16.5" customHeight="1"/>
+    <row r="411" ht="16.5" customHeight="1"/>
+    <row r="412" ht="16.5" customHeight="1"/>
+    <row r="413" ht="16.5" customHeight="1"/>
+    <row r="414" ht="16.5" customHeight="1"/>
+    <row r="415" ht="16.5" customHeight="1"/>
+    <row r="416" ht="16.5" customHeight="1"/>
+    <row r="417" ht="16.5" customHeight="1"/>
+    <row r="418" ht="16.5" customHeight="1"/>
+    <row r="419" ht="16.5" customHeight="1"/>
+    <row r="420" ht="16.5" customHeight="1"/>
+    <row r="421" ht="16.5" customHeight="1"/>
+    <row r="422" ht="16.5" customHeight="1"/>
+    <row r="423" ht="16.5" customHeight="1"/>
+    <row r="424" ht="16.5" customHeight="1"/>
+    <row r="425" ht="16.5" customHeight="1"/>
+    <row r="426" ht="16.5" customHeight="1"/>
+    <row r="427" ht="16.5" customHeight="1"/>
+    <row r="428" ht="16.5" customHeight="1"/>
+    <row r="429" ht="16.5" customHeight="1"/>
+    <row r="430" ht="16.5" customHeight="1"/>
+    <row r="431" ht="16.5" customHeight="1"/>
+    <row r="432" ht="16.5" customHeight="1"/>
+    <row r="433" ht="16.5" customHeight="1"/>
+    <row r="434" ht="16.5" customHeight="1"/>
+    <row r="435" ht="16.5" customHeight="1"/>
+    <row r="436" ht="16.5" customHeight="1"/>
+    <row r="437" ht="16.5" customHeight="1"/>
+    <row r="438" ht="16.5" customHeight="1"/>
+    <row r="439" ht="16.5" customHeight="1"/>
+    <row r="440" ht="16.5" customHeight="1"/>
+    <row r="441" ht="16.5" customHeight="1"/>
+    <row r="442" ht="16.5" customHeight="1"/>
+    <row r="443" ht="16.5" customHeight="1"/>
+    <row r="444" ht="16.5" customHeight="1"/>
+    <row r="445" ht="16.5" customHeight="1"/>
+    <row r="446" ht="16.5" customHeight="1"/>
+    <row r="447" ht="16.5" customHeight="1"/>
+    <row r="448" ht="16.5" customHeight="1"/>
+    <row r="449" ht="16.5" customHeight="1"/>
+    <row r="450" ht="16.5" customHeight="1"/>
+    <row r="451" ht="16.5" customHeight="1"/>
+    <row r="452" ht="16.5" customHeight="1"/>
+    <row r="453" ht="16.5" customHeight="1"/>
+    <row r="454" ht="16.5" customHeight="1"/>
+    <row r="455" ht="16.5" customHeight="1"/>
+    <row r="456" ht="16.5" customHeight="1"/>
+    <row r="457" ht="16.5" customHeight="1"/>
+    <row r="458" ht="16.5" customHeight="1"/>
+    <row r="459" ht="16.5" customHeight="1"/>
+    <row r="460" ht="16.5" customHeight="1"/>
+    <row r="461" ht="16.5" customHeight="1"/>
+    <row r="462" ht="16.5" customHeight="1"/>
+    <row r="463" ht="16.5" customHeight="1"/>
+    <row r="464" ht="16.5" customHeight="1"/>
+    <row r="465" ht="16.5" customHeight="1"/>
+    <row r="466" ht="16.5" customHeight="1"/>
+    <row r="467" ht="16.5" customHeight="1"/>
+    <row r="468" ht="16.5" customHeight="1"/>
+    <row r="469" ht="16.5" customHeight="1"/>
+    <row r="470" ht="16.5" customHeight="1"/>
+    <row r="471" ht="16.5" customHeight="1"/>
+    <row r="472" ht="16.5" customHeight="1"/>
+    <row r="473" ht="16.5" customHeight="1"/>
+    <row r="474" ht="16.5" customHeight="1"/>
+    <row r="475" ht="16.5" customHeight="1"/>
+    <row r="476" ht="16.5" customHeight="1"/>
+    <row r="477" ht="16.5" customHeight="1"/>
+    <row r="478" ht="16.5" customHeight="1"/>
+    <row r="479" ht="16.5" customHeight="1"/>
+    <row r="480" ht="16.5" customHeight="1"/>
+    <row r="481" ht="16.5" customHeight="1"/>
+    <row r="482" ht="16.5" customHeight="1"/>
+    <row r="483" ht="16.5" customHeight="1"/>
+    <row r="484" ht="16.5" customHeight="1"/>
+    <row r="485" ht="16.5" customHeight="1"/>
+    <row r="486" ht="16.5" customHeight="1"/>
+    <row r="487" ht="16.5" customHeight="1"/>
+    <row r="488" ht="16.5" customHeight="1"/>
+    <row r="489" ht="16.5" customHeight="1"/>
+    <row r="490" ht="16.5" customHeight="1"/>
+    <row r="491" ht="16.5" customHeight="1"/>
+    <row r="492" ht="16.5" customHeight="1"/>
+    <row r="493" ht="16.5" customHeight="1"/>
+    <row r="494" ht="16.5" customHeight="1"/>
+    <row r="495" ht="16.5" customHeight="1"/>
+    <row r="496" ht="16.5" customHeight="1"/>
+    <row r="497" ht="16.5" customHeight="1"/>
+    <row r="498" ht="16.5" customHeight="1"/>
+    <row r="499" ht="16.5" customHeight="1"/>
+    <row r="500" ht="16.5" customHeight="1"/>
+    <row r="501" ht="16.5" customHeight="1"/>
+    <row r="502" ht="16.5" customHeight="1"/>
+    <row r="503" ht="16.5" customHeight="1"/>
+    <row r="504" ht="16.5" customHeight="1"/>
+    <row r="505" ht="16.5" customHeight="1"/>
+    <row r="506" ht="16.5" customHeight="1"/>
+    <row r="507" ht="16.5" customHeight="1"/>
+    <row r="508" ht="16.5" customHeight="1"/>
+    <row r="509" ht="16.5" customHeight="1"/>
+    <row r="510" ht="16.5" customHeight="1"/>
+    <row r="511" ht="16.5" customHeight="1"/>
+    <row r="512" ht="16.5" customHeight="1"/>
+    <row r="513" ht="16.5" customHeight="1"/>
+    <row r="514" ht="16.5" customHeight="1"/>
+    <row r="515" ht="16.5" customHeight="1"/>
+    <row r="516" ht="16.5" customHeight="1"/>
+    <row r="517" ht="16.5" customHeight="1"/>
+    <row r="518" ht="16.5" customHeight="1"/>
+    <row r="519" ht="16.5" customHeight="1"/>
+    <row r="520" ht="16.5" customHeight="1"/>
+    <row r="521" ht="16.5" customHeight="1"/>
+    <row r="522" ht="16.5" customHeight="1"/>
+    <row r="523" ht="16.5" customHeight="1"/>
+    <row r="524" ht="16.5" customHeight="1"/>
+    <row r="525" ht="16.5" customHeight="1"/>
+    <row r="526" ht="16.5" customHeight="1"/>
+    <row r="527" ht="16.5" customHeight="1"/>
+    <row r="528" ht="16.5" customHeight="1"/>
+    <row r="529" ht="16.5" customHeight="1"/>
+    <row r="530" ht="16.5" customHeight="1"/>
+    <row r="531" ht="16.5" customHeight="1"/>
+    <row r="532" ht="16.5" customHeight="1"/>
+    <row r="533" ht="16.5" customHeight="1"/>
+    <row r="534" ht="16.5" customHeight="1"/>
+    <row r="535" ht="16.5" customHeight="1"/>
+    <row r="536" ht="16.5" customHeight="1"/>
+    <row r="537" ht="16.5" customHeight="1"/>
+    <row r="538" ht="16.5" customHeight="1"/>
+    <row r="539" ht="16.5" customHeight="1"/>
+    <row r="540" ht="16.5" customHeight="1"/>
+    <row r="541" ht="16.5" customHeight="1"/>
+    <row r="542" ht="16.5" customHeight="1"/>
+    <row r="543" ht="16.5" customHeight="1"/>
+    <row r="544" ht="16.5" customHeight="1"/>
+    <row r="545" ht="16.5" customHeight="1"/>
+    <row r="546" ht="16.5" customHeight="1"/>
+    <row r="547" ht="16.5" customHeight="1"/>
+    <row r="548" ht="16.5" customHeight="1"/>
+    <row r="549" ht="16.5" customHeight="1"/>
+    <row r="550" ht="16.5" customHeight="1"/>
+    <row r="551" ht="16.5" customHeight="1"/>
+    <row r="552" ht="16.5" customHeight="1"/>
+    <row r="553" ht="16.5" customHeight="1"/>
+    <row r="554" ht="16.5" customHeight="1"/>
+    <row r="555" ht="16.5" customHeight="1"/>
+    <row r="556" ht="16.5" customHeight="1"/>
+    <row r="557" ht="16.5" customHeight="1"/>
+    <row r="558" ht="16.5" customHeight="1"/>
+    <row r="559" ht="16.5" customHeight="1"/>
+    <row r="560" ht="16.5" customHeight="1"/>
+    <row r="561" ht="16.5" customHeight="1"/>
+    <row r="562" ht="16.5" customHeight="1"/>
+    <row r="563" ht="16.5" customHeight="1"/>
+    <row r="564" ht="16.5" customHeight="1"/>
+    <row r="565" ht="16.5" customHeight="1"/>
+    <row r="566" ht="16.5" customHeight="1"/>
+    <row r="567" ht="16.5" customHeight="1"/>
+    <row r="568" ht="16.5" customHeight="1"/>
+    <row r="569" ht="16.5" customHeight="1"/>
+    <row r="570" ht="16.5" customHeight="1"/>
+    <row r="571" ht="16.5" customHeight="1"/>
+    <row r="572" ht="16.5" customHeight="1"/>
+    <row r="573" ht="16.5" customHeight="1"/>
+    <row r="574" ht="16.5" customHeight="1"/>
+    <row r="575" ht="16.5" customHeight="1"/>
+    <row r="576" ht="16.5" customHeight="1"/>
+    <row r="577" ht="16.5" customHeight="1"/>
+    <row r="578" ht="16.5" customHeight="1"/>
+    <row r="579" ht="16.5" customHeight="1"/>
+    <row r="580" ht="16.5" customHeight="1"/>
+    <row r="581" ht="16.5" customHeight="1"/>
+    <row r="582" ht="16.5" customHeight="1"/>
+    <row r="583" ht="16.5" customHeight="1"/>
+    <row r="584" ht="16.5" customHeight="1"/>
+    <row r="585" ht="16.5" customHeight="1"/>
+    <row r="586" ht="16.5" customHeight="1"/>
+    <row r="587" ht="16.5" customHeight="1"/>
+    <row r="588" ht="16.5" customHeight="1"/>
+    <row r="589" ht="16.5" customHeight="1"/>
+    <row r="590" ht="16.5" customHeight="1"/>
+    <row r="591" ht="16.5" customHeight="1"/>
+    <row r="592" ht="16.5" customHeight="1"/>
+    <row r="593" ht="16.5" customHeight="1"/>
+    <row r="594" ht="16.5" customHeight="1"/>
+    <row r="595" ht="16.5" customHeight="1"/>
+    <row r="596" ht="16.5" customHeight="1"/>
+    <row r="597" ht="16.5" customHeight="1"/>
+    <row r="598" ht="16.5" customHeight="1"/>
+    <row r="599" ht="16.5" customHeight="1"/>
+    <row r="600" ht="16.5" customHeight="1"/>
+    <row r="601" ht="16.5" customHeight="1"/>
+    <row r="602" ht="16.5" customHeight="1"/>
+    <row r="603" ht="16.5" customHeight="1"/>
+    <row r="604" ht="16.5" customHeight="1"/>
+    <row r="605" ht="16.5" customHeight="1"/>
+    <row r="606" ht="16.5" customHeight="1"/>
+    <row r="607" ht="16.5" customHeight="1"/>
+    <row r="608" ht="16.5" customHeight="1"/>
+    <row r="609" ht="16.5" customHeight="1"/>
+    <row r="610" ht="16.5" customHeight="1"/>
+    <row r="611" ht="16.5" customHeight="1"/>
+    <row r="612" ht="16.5" customHeight="1"/>
+    <row r="613" ht="16.5" customHeight="1"/>
+    <row r="614" ht="16.5" customHeight="1"/>
+    <row r="615" ht="16.5" customHeight="1"/>
+    <row r="616" ht="16.5" customHeight="1"/>
+    <row r="617" ht="16.5" customHeight="1"/>
+    <row r="618" ht="16.5" customHeight="1"/>
+    <row r="619" ht="16.5" customHeight="1"/>
+    <row r="620" ht="16.5" customHeight="1"/>
+    <row r="621" ht="16.5" customHeight="1"/>
+    <row r="622" ht="16.5" customHeight="1"/>
+    <row r="623" ht="16.5" customHeight="1"/>
+    <row r="624" ht="16.5" customHeight="1"/>
+    <row r="625" ht="16.5" customHeight="1"/>
+    <row r="626" ht="16.5" customHeight="1"/>
+    <row r="627" ht="16.5" customHeight="1"/>
+    <row r="628" ht="16.5" customHeight="1"/>
+    <row r="629" ht="16.5" customHeight="1"/>
+    <row r="630" ht="16.5" customHeight="1"/>
+    <row r="631" ht="16.5" customHeight="1"/>
+    <row r="632" ht="16.5" customHeight="1"/>
+    <row r="633" ht="16.5" customHeight="1"/>
+    <row r="634" ht="16.5" customHeight="1"/>
+    <row r="635" ht="16.5" customHeight="1"/>
+    <row r="636" ht="16.5" customHeight="1"/>
+    <row r="637" ht="16.5" customHeight="1"/>
+    <row r="638" ht="16.5" customHeight="1"/>
+    <row r="639" ht="16.5" customHeight="1"/>
+    <row r="640" ht="16.5" customHeight="1"/>
+    <row r="641" ht="16.5" customHeight="1"/>
+    <row r="642" ht="16.5" customHeight="1"/>
+    <row r="643" ht="16.5" customHeight="1"/>
+    <row r="644" ht="16.5" customHeight="1"/>
+    <row r="645" ht="16.5" customHeight="1"/>
+    <row r="646" ht="16.5" customHeight="1"/>
+    <row r="647" ht="16.5" customHeight="1"/>
+    <row r="648" ht="16.5" customHeight="1"/>
+    <row r="649" ht="16.5" customHeight="1"/>
+    <row r="650" ht="16.5" customHeight="1"/>
+    <row r="651" ht="16.5" customHeight="1"/>
+    <row r="652" ht="16.5" customHeight="1"/>
+    <row r="653" ht="16.5" customHeight="1"/>
+    <row r="654" ht="16.5" customHeight="1"/>
+    <row r="655" ht="16.5" customHeight="1"/>
+    <row r="656" ht="16.5" customHeight="1"/>
+    <row r="657" ht="16.5" customHeight="1"/>
+    <row r="658" ht="16.5" customHeight="1"/>
+    <row r="659" ht="16.5" customHeight="1"/>
+    <row r="660" ht="16.5" customHeight="1"/>
+    <row r="661" ht="16.5" customHeight="1"/>
+    <row r="662" ht="16.5" customHeight="1"/>
+    <row r="663" ht="16.5" customHeight="1"/>
+    <row r="664" ht="16.5" customHeight="1"/>
+    <row r="665" ht="16.5" customHeight="1"/>
+    <row r="666" ht="16.5" customHeight="1"/>
+    <row r="667" ht="16.5" customHeight="1"/>
+    <row r="668" ht="16.5" customHeight="1"/>
+    <row r="669" ht="16.5" customHeight="1"/>
+    <row r="670" ht="16.5" customHeight="1"/>
+    <row r="671" ht="16.5" customHeight="1"/>
+    <row r="672" ht="16.5" customHeight="1"/>
+    <row r="673" ht="16.5" customHeight="1"/>
+    <row r="674" ht="16.5" customHeight="1"/>
+    <row r="675" ht="16.5" customHeight="1"/>
+    <row r="676" ht="16.5" customHeight="1"/>
+    <row r="677" ht="16.5" customHeight="1"/>
+    <row r="678" ht="16.5" customHeight="1"/>
+    <row r="679" ht="16.5" customHeight="1"/>
+    <row r="680" ht="16.5" customHeight="1"/>
+    <row r="681" ht="16.5" customHeight="1"/>
+    <row r="682" ht="16.5" customHeight="1"/>
+    <row r="683" ht="16.5" customHeight="1"/>
+    <row r="684" ht="16.5" customHeight="1"/>
+    <row r="685" ht="16.5" customHeight="1"/>
+    <row r="686" ht="16.5" customHeight="1"/>
+    <row r="687" ht="16.5" customHeight="1"/>
+    <row r="688" ht="16.5" customHeight="1"/>
+    <row r="689" ht="16.5" customHeight="1"/>
+    <row r="690" ht="16.5" customHeight="1"/>
+    <row r="691" ht="16.5" customHeight="1"/>
+    <row r="692" ht="16.5" customHeight="1"/>
+    <row r="693" ht="16.5" customHeight="1"/>
+    <row r="694" ht="16.5" customHeight="1"/>
+    <row r="695" ht="16.5" customHeight="1"/>
+    <row r="696" ht="16.5" customHeight="1"/>
+    <row r="697" ht="16.5" customHeight="1"/>
+    <row r="698" ht="16.5" customHeight="1"/>
+    <row r="699" ht="16.5" customHeight="1"/>
+    <row r="700" ht="16.5" customHeight="1"/>
+    <row r="701" ht="16.5" customHeight="1"/>
+    <row r="702" ht="16.5" customHeight="1"/>
+    <row r="703" ht="16.5" customHeight="1"/>
+    <row r="704" ht="16.5" customHeight="1"/>
+    <row r="705" ht="16.5" customHeight="1"/>
+    <row r="706" ht="16.5" customHeight="1"/>
+    <row r="707" ht="16.5" customHeight="1"/>
+    <row r="708" ht="16.5" customHeight="1"/>
+    <row r="709" ht="16.5" customHeight="1"/>
+    <row r="710" ht="16.5" customHeight="1"/>
+    <row r="711" ht="16.5" customHeight="1"/>
+    <row r="712" ht="16.5" customHeight="1"/>
+    <row r="713" ht="16.5" customHeight="1"/>
+    <row r="714" ht="16.5" customHeight="1"/>
+    <row r="715" ht="16.5" customHeight="1"/>
+    <row r="716" ht="16.5" customHeight="1"/>
+    <row r="717" ht="16.5" customHeight="1"/>
+    <row r="718" ht="16.5" customHeight="1"/>
+    <row r="719" ht="16.5" customHeight="1"/>
+    <row r="720" ht="16.5" customHeight="1"/>
+    <row r="721" ht="16.5" customHeight="1"/>
+    <row r="722" ht="16.5" customHeight="1"/>
+    <row r="723" ht="16.5" customHeight="1"/>
+    <row r="724" ht="16.5" customHeight="1"/>
+    <row r="725" ht="16.5" customHeight="1"/>
+    <row r="726" ht="16.5" customHeight="1"/>
+    <row r="727" ht="16.5" customHeight="1"/>
+    <row r="728" ht="16.5" customHeight="1"/>
+    <row r="729" ht="16.5" customHeight="1"/>
+    <row r="730" ht="16.5" customHeight="1"/>
+    <row r="731" ht="16.5" customHeight="1"/>
+    <row r="732" ht="16.5" customHeight="1"/>
+    <row r="733" ht="16.5" customHeight="1"/>
+    <row r="734" ht="16.5" customHeight="1"/>
+    <row r="735" ht="16.5" customHeight="1"/>
+    <row r="736" ht="16.5" customHeight="1"/>
+    <row r="737" ht="16.5" customHeight="1"/>
+    <row r="738" ht="16.5" customHeight="1"/>
+    <row r="739" ht="16.5" customHeight="1"/>
+    <row r="740" ht="16.5" customHeight="1"/>
+    <row r="741" ht="16.5" customHeight="1"/>
+    <row r="742" ht="16.5" customHeight="1"/>
+    <row r="743" ht="16.5" customHeight="1"/>
+    <row r="744" ht="16.5" customHeight="1"/>
+    <row r="745" ht="16.5" customHeight="1"/>
+    <row r="746" ht="16.5" customHeight="1"/>
+    <row r="747" ht="16.5" customHeight="1"/>
+    <row r="748" ht="16.5" customHeight="1"/>
+    <row r="749" ht="16.5" customHeight="1"/>
+    <row r="750" ht="16.5" customHeight="1"/>
+    <row r="751" ht="16.5" customHeight="1"/>
+    <row r="752" ht="16.5" customHeight="1"/>
+    <row r="753" ht="16.5" customHeight="1"/>
+    <row r="754" ht="16.5" customHeight="1"/>
+    <row r="755" ht="16.5" customHeight="1"/>
+    <row r="756" ht="16.5" customHeight="1"/>
+    <row r="757" ht="16.5" customHeight="1"/>
+    <row r="758" ht="16.5" customHeight="1"/>
+    <row r="759" ht="16.5" customHeight="1"/>
+    <row r="760" ht="16.5" customHeight="1"/>
+    <row r="761" ht="16.5" customHeight="1"/>
+    <row r="762" ht="16.5" customHeight="1"/>
+    <row r="763" ht="16.5" customHeight="1"/>
+    <row r="764" ht="16.5" customHeight="1"/>
+    <row r="765" ht="16.5" customHeight="1"/>
+    <row r="766" ht="16.5" customHeight="1"/>
+    <row r="767" ht="16.5" customHeight="1"/>
+    <row r="768" ht="16.5" customHeight="1"/>
+    <row r="769" ht="16.5" customHeight="1"/>
+    <row r="770" ht="16.5" customHeight="1"/>
+    <row r="771" ht="16.5" customHeight="1"/>
+    <row r="772" ht="16.5" customHeight="1"/>
+    <row r="773" ht="16.5" customHeight="1"/>
+    <row r="774" ht="16.5" customHeight="1"/>
+    <row r="775" ht="16.5" customHeight="1"/>
+    <row r="776" ht="16.5" customHeight="1"/>
+    <row r="777" ht="16.5" customHeight="1"/>
+    <row r="778" ht="16.5" customHeight="1"/>
+    <row r="779" ht="16.5" customHeight="1"/>
+    <row r="780" ht="16.5" customHeight="1"/>
+    <row r="781" ht="16.5" customHeight="1"/>
+    <row r="782" ht="16.5" customHeight="1"/>
+    <row r="783" ht="16.5" customHeight="1"/>
+    <row r="784" ht="16.5" customHeight="1"/>
+    <row r="785" ht="16.5" customHeight="1"/>
+    <row r="786" ht="16.5" customHeight="1"/>
+    <row r="787" ht="16.5" customHeight="1"/>
+    <row r="788" ht="16.5" customHeight="1"/>
+    <row r="789" ht="16.5" customHeight="1"/>
+    <row r="790" ht="16.5" customHeight="1"/>
+    <row r="791" ht="16.5" customHeight="1"/>
+    <row r="792" ht="16.5" customHeight="1"/>
+    <row r="793" ht="16.5" customHeight="1"/>
+    <row r="794" ht="16.5" customHeight="1"/>
+    <row r="795" ht="16.5" customHeight="1"/>
+    <row r="796" ht="16.5" customHeight="1"/>
+    <row r="797" ht="16.5" customHeight="1"/>
+    <row r="798" ht="16.5" customHeight="1"/>
+    <row r="799" ht="16.5" customHeight="1"/>
+    <row r="800" ht="16.5" customHeight="1"/>
+    <row r="801" ht="16.5" customHeight="1"/>
+    <row r="802" ht="16.5" customHeight="1"/>
+    <row r="803" ht="16.5" customHeight="1"/>
+    <row r="804" ht="16.5" customHeight="1"/>
+    <row r="805" ht="16.5" customHeight="1"/>
+    <row r="806" ht="16.5" customHeight="1"/>
+    <row r="807" ht="16.5" customHeight="1"/>
+    <row r="808" ht="16.5" customHeight="1"/>
+    <row r="809" ht="16.5" customHeight="1"/>
+    <row r="810" ht="16.5" customHeight="1"/>
+    <row r="811" ht="16.5" customHeight="1"/>
+    <row r="812" ht="16.5" customHeight="1"/>
+    <row r="813" ht="16.5" customHeight="1"/>
+    <row r="814" ht="16.5" customHeight="1"/>
+    <row r="815" ht="16.5" customHeight="1"/>
+    <row r="816" ht="16.5" customHeight="1"/>
+    <row r="817" ht="16.5" customHeight="1"/>
+    <row r="818" ht="16.5" customHeight="1"/>
+    <row r="819" ht="16.5" customHeight="1"/>
+    <row r="820" ht="16.5" customHeight="1"/>
+    <row r="821" ht="16.5" customHeight="1"/>
+    <row r="822" ht="16.5" customHeight="1"/>
+    <row r="823" ht="16.5" customHeight="1"/>
+    <row r="824" ht="16.5" customHeight="1"/>
+    <row r="825" ht="16.5" customHeight="1"/>
+    <row r="826" ht="16.5" customHeight="1"/>
+    <row r="827" ht="16.5" customHeight="1"/>
+    <row r="828" ht="16.5" customHeight="1"/>
+    <row r="829" ht="16.5" customHeight="1"/>
+    <row r="830" ht="16.5" customHeight="1"/>
+    <row r="831" ht="16.5" customHeight="1"/>
+    <row r="832" ht="16.5" customHeight="1"/>
+    <row r="833" ht="16.5" customHeight="1"/>
+    <row r="834" ht="16.5" customHeight="1"/>
+    <row r="835" ht="16.5" customHeight="1"/>
+    <row r="836" ht="16.5" customHeight="1"/>
+    <row r="837" ht="16.5" customHeight="1"/>
+    <row r="838" ht="16.5" customHeight="1"/>
+    <row r="839" ht="16.5" customHeight="1"/>
+    <row r="840" ht="16.5" customHeight="1"/>
+    <row r="841" ht="16.5" customHeight="1"/>
+    <row r="842" ht="16.5" customHeight="1"/>
+    <row r="843" ht="16.5" customHeight="1"/>
+    <row r="844" ht="16.5" customHeight="1"/>
+    <row r="845" ht="16.5" customHeight="1"/>
+    <row r="846" ht="16.5" customHeight="1"/>
+    <row r="847" ht="16.5" customHeight="1"/>
+    <row r="848" ht="16.5" customHeight="1"/>
+    <row r="849" ht="16.5" customHeight="1"/>
+    <row r="850" ht="16.5" customHeight="1"/>
+    <row r="851" ht="16.5" customHeight="1"/>
+    <row r="852" ht="16.5" customHeight="1"/>
+    <row r="853" ht="16.5" customHeight="1"/>
+    <row r="854" ht="16.5" customHeight="1"/>
+    <row r="855" ht="16.5" customHeight="1"/>
+    <row r="856" ht="16.5" customHeight="1"/>
+    <row r="857" ht="16.5" customHeight="1"/>
+    <row r="858" ht="16.5" customHeight="1"/>
+    <row r="859" ht="16.5" customHeight="1"/>
+    <row r="860" ht="16.5" customHeight="1"/>
+    <row r="861" ht="16.5" customHeight="1"/>
+    <row r="862" ht="16.5" customHeight="1"/>
+    <row r="863" ht="16.5" customHeight="1"/>
+    <row r="864" ht="16.5" customHeight="1"/>
+    <row r="865" ht="16.5" customHeight="1"/>
+    <row r="866" ht="16.5" customHeight="1"/>
+    <row r="867" ht="16.5" customHeight="1"/>
+    <row r="868" ht="16.5" customHeight="1"/>
+    <row r="869" ht="16.5" customHeight="1"/>
+    <row r="870" ht="16.5" customHeight="1"/>
+    <row r="871" ht="16.5" customHeight="1"/>
+    <row r="872" ht="16.5" customHeight="1"/>
+    <row r="873" ht="16.5" customHeight="1"/>
+    <row r="874" ht="16.5" customHeight="1"/>
+    <row r="875" ht="16.5" customHeight="1"/>
+    <row r="876" ht="16.5" customHeight="1"/>
+    <row r="877" ht="16.5" customHeight="1"/>
+    <row r="878" ht="16.5" customHeight="1"/>
+    <row r="879" ht="16.5" customHeight="1"/>
+    <row r="880" ht="16.5" customHeight="1"/>
+    <row r="881" ht="16.5" customHeight="1"/>
+    <row r="882" ht="16.5" customHeight="1"/>
+    <row r="883" ht="16.5" customHeight="1"/>
+    <row r="884" ht="16.5" customHeight="1"/>
+    <row r="885" ht="16.5" customHeight="1"/>
+    <row r="886" ht="16.5" customHeight="1"/>
+    <row r="887" ht="16.5" customHeight="1"/>
+    <row r="888" ht="16.5" customHeight="1"/>
+    <row r="889" ht="16.5" customHeight="1"/>
+    <row r="890" ht="16.5" customHeight="1"/>
+    <row r="891" ht="16.5" customHeight="1"/>
+    <row r="892" ht="16.5" customHeight="1"/>
+    <row r="893" ht="16.5" customHeight="1"/>
+    <row r="894" ht="16.5" customHeight="1"/>
+    <row r="895" ht="16.5" customHeight="1"/>
+    <row r="896" ht="16.5" customHeight="1"/>
+    <row r="897" ht="16.5" customHeight="1"/>
+    <row r="898" ht="16.5" customHeight="1"/>
+    <row r="899" ht="16.5" customHeight="1"/>
+    <row r="900" ht="16.5" customHeight="1"/>
+    <row r="901" ht="16.5" customHeight="1"/>
+    <row r="902" ht="16.5" customHeight="1"/>
+    <row r="903" ht="16.5" customHeight="1"/>
+    <row r="904" ht="16.5" customHeight="1"/>
+    <row r="905" ht="16.5" customHeight="1"/>
+    <row r="906" ht="16.5" customHeight="1"/>
+    <row r="907" ht="16.5" customHeight="1"/>
+    <row r="908" ht="16.5" customHeight="1"/>
+    <row r="909" ht="16.5" customHeight="1"/>
+    <row r="910" ht="16.5" customHeight="1"/>
+    <row r="911" ht="16.5" customHeight="1"/>
+    <row r="912" ht="16.5" customHeight="1"/>
+    <row r="913" ht="16.5" customHeight="1"/>
+    <row r="914" ht="16.5" customHeight="1"/>
+    <row r="915" ht="16.5" customHeight="1"/>
+    <row r="916" ht="16.5" customHeight="1"/>
+    <row r="917" ht="16.5" customHeight="1"/>
+    <row r="918" ht="16.5" customHeight="1"/>
+    <row r="919" ht="16.5" customHeight="1"/>
+    <row r="920" ht="16.5" customHeight="1"/>
+    <row r="921" ht="16.5" customHeight="1"/>
+    <row r="922" ht="16.5" customHeight="1"/>
+    <row r="923" ht="16.5" customHeight="1"/>
+    <row r="924" ht="16.5" customHeight="1"/>
+    <row r="925" ht="16.5" customHeight="1"/>
+    <row r="926" ht="16.5" customHeight="1"/>
+    <row r="927" ht="16.5" customHeight="1"/>
+    <row r="928" ht="16.5" customHeight="1"/>
+    <row r="929" ht="16.5" customHeight="1"/>
+    <row r="930" ht="16.5" customHeight="1"/>
+    <row r="931" ht="16.5" customHeight="1"/>
+    <row r="932" ht="16.5" customHeight="1"/>
+    <row r="933" ht="16.5" customHeight="1"/>
+    <row r="934" ht="16.5" customHeight="1"/>
+    <row r="935" ht="16.5" customHeight="1"/>
+    <row r="936" ht="16.5" customHeight="1"/>
+    <row r="937" ht="16.5" customHeight="1"/>
+    <row r="938" ht="16.5" customHeight="1"/>
+    <row r="939" ht="16.5" customHeight="1"/>
+    <row r="940" ht="16.5" customHeight="1"/>
+    <row r="941" ht="16.5" customHeight="1"/>
+    <row r="942" ht="16.5" customHeight="1"/>
+    <row r="943" ht="16.5" customHeight="1"/>
+    <row r="944" ht="16.5" customHeight="1"/>
+    <row r="945" ht="16.5" customHeight="1"/>
+    <row r="946" ht="16.5" customHeight="1"/>
+    <row r="947" ht="16.5" customHeight="1"/>
+    <row r="948" ht="16.5" customHeight="1"/>
+    <row r="949" ht="16.5" customHeight="1"/>
+    <row r="950" ht="16.5" customHeight="1"/>
+    <row r="951" ht="16.5" customHeight="1"/>
+    <row r="952" ht="16.5" customHeight="1"/>
+    <row r="953" ht="16.5" customHeight="1"/>
+    <row r="954" ht="16.5" customHeight="1"/>
+    <row r="955" ht="16.5" customHeight="1"/>
+    <row r="956" ht="16.5" customHeight="1"/>
+    <row r="957" ht="16.5" customHeight="1"/>
+    <row r="958" ht="16.5" customHeight="1"/>
+    <row r="959" ht="16.5" customHeight="1"/>
+    <row r="960" ht="16.5" customHeight="1"/>
+    <row r="961" ht="16.5" customHeight="1"/>
+    <row r="962" ht="16.5" customHeight="1"/>
+    <row r="963" ht="16.5" customHeight="1"/>
+    <row r="964" ht="16.5" customHeight="1"/>
+    <row r="965" ht="16.5" customHeight="1"/>
+    <row r="966" ht="16.5" customHeight="1"/>
+    <row r="967" ht="16.5" customHeight="1"/>
+    <row r="968" ht="16.5" customHeight="1"/>
+    <row r="969" ht="16.5" customHeight="1"/>
+    <row r="970" ht="16.5" customHeight="1"/>
+    <row r="971" ht="16.5" customHeight="1"/>
+    <row r="972" ht="16.5" customHeight="1"/>
+    <row r="973" ht="16.5" customHeight="1"/>
+    <row r="974" ht="16.5" customHeight="1"/>
+    <row r="975" ht="16.5" customHeight="1"/>
+    <row r="976" ht="16.5" customHeight="1"/>
+    <row r="977" ht="16.5" customHeight="1"/>
+    <row r="978" ht="16.5" customHeight="1"/>
+    <row r="979" ht="16.5" customHeight="1"/>
+    <row r="980" ht="16.5" customHeight="1"/>
+    <row r="981" ht="16.5" customHeight="1"/>
+    <row r="982" ht="16.5" customHeight="1"/>
+    <row r="983" ht="16.5" customHeight="1"/>
+    <row r="984" ht="16.5" customHeight="1"/>
+    <row r="985" ht="16.5" customHeight="1"/>
+    <row r="986" ht="16.5" customHeight="1"/>
+    <row r="987" ht="16.5" customHeight="1"/>
+    <row r="988" ht="16.5" customHeight="1"/>
+    <row r="989" ht="16.5" customHeight="1"/>
+    <row r="990" ht="16.5" customHeight="1"/>
+    <row r="991" ht="16.5" customHeight="1"/>
+    <row r="992" ht="16.5" customHeight="1"/>
+    <row r="993" ht="16.5" customHeight="1"/>
+    <row r="994" ht="16.5" customHeight="1"/>
+    <row r="995" ht="16.5" customHeight="1"/>
+    <row r="996" ht="16.5" customHeight="1"/>
+    <row r="997" ht="16.5" customHeight="1"/>
+    <row r="998" ht="16.5" customHeight="1"/>
+    <row r="999" ht="16.5" customHeight="1"/>
+    <row r="1000" ht="16.5" customHeight="1"/>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Fix] ExcelData, GameScene UI
데이터 수정( 임시데이터 추가 - 버프, 몬스터, 스킬)

게임씬 UI 승리, 패배 시 UI 수정
</commit_message>
<xml_diff>
--- a/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
+++ b/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="1650" windowWidth="21600" windowHeight="11385" tabRatio="500"/>
+    <workbookView xWindow="6840" yWindow="1650" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
     <sheet name="Skills" sheetId="2" r:id="rId2"/>
     <sheet name="Monsters" sheetId="3" r:id="rId3"/>
     <sheet name="Items" sheetId="4" r:id="rId4"/>
-    <sheet name="BUFF" sheetId="6" r:id="rId5"/>
+    <sheet name="Buff" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="81">
   <si>
     <t>job</t>
   </si>
@@ -398,18 +398,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>상승치</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>스텟</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>패자의 분노</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -426,10 +414,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>조건</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>레드 몬스터 처치 시</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -438,14 +422,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>ATK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DEF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>에픽</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -454,14 +430,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>ATK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SPD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>파이어볼</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -483,6 +451,42 @@
   </si>
   <si>
     <t>은신</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>info</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>atk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>def</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>spd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>설명</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cooltime</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>condition</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -834,7 +838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -2009,10 +2013,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1000"/>
+  <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2025,7 +2029,7 @@
     <col min="27" max="1025" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" customHeight="1">
+    <row r="1" spans="1:7" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2038,8 +2042,17 @@
       <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" customHeight="1">
+    <row r="2" spans="1:7" ht="16.5" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -2052,8 +2065,17 @@
       <c r="D2" s="4">
         <v>2</v>
       </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5" customHeight="1">
+    <row r="3" spans="1:7" ht="16.5" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -2066,8 +2088,17 @@
       <c r="D3" s="4">
         <v>3</v>
       </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" customHeight="1">
+    <row r="4" spans="1:7" ht="16.5" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2080,13 +2111,22 @@
       <c r="D4" s="4">
         <v>3</v>
       </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" ht="16.5" customHeight="1">
+    <row r="5" spans="1:7" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>47</v>
@@ -2094,13 +2134,22 @@
       <c r="D5" s="4">
         <v>3</v>
       </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" ht="16.5" customHeight="1">
+    <row r="6" spans="1:7" ht="16.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>47</v>
@@ -2108,13 +2157,22 @@
       <c r="D6" s="4">
         <v>3</v>
       </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" ht="16.5" customHeight="1">
+    <row r="7" spans="1:7" ht="16.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>47</v>
@@ -2122,13 +2180,22 @@
       <c r="D7" s="4">
         <v>3</v>
       </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" ht="16.5" customHeight="1">
+    <row r="8" spans="1:7" ht="16.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>47</v>
@@ -2136,27 +2203,45 @@
       <c r="D8" s="4">
         <v>3</v>
       </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" ht="16.5" customHeight="1">
+    <row r="9" spans="1:7" ht="16.5" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="D9" s="4">
         <v>3</v>
       </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" ht="16.5" customHeight="1">
+    <row r="10" spans="1:7" ht="16.5" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>47</v>
@@ -2164,13 +2249,22 @@
       <c r="D10" s="4">
         <v>3</v>
       </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" ht="16.5" customHeight="1"/>
-    <row r="12" spans="1:4" ht="16.5" customHeight="1"/>
-    <row r="13" spans="1:4" ht="16.5" customHeight="1"/>
-    <row r="14" spans="1:4" ht="16.5" customHeight="1"/>
-    <row r="15" spans="1:4" ht="16.5" customHeight="1"/>
-    <row r="16" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="11" spans="1:7" ht="16.5" customHeight="1"/>
+    <row r="12" spans="1:7" ht="16.5" customHeight="1"/>
+    <row r="13" spans="1:7" ht="16.5" customHeight="1"/>
+    <row r="14" spans="1:7" ht="16.5" customHeight="1"/>
+    <row r="15" spans="1:7" ht="16.5" customHeight="1"/>
+    <row r="16" spans="1:7" ht="16.5" customHeight="1"/>
     <row r="17" ht="16.5" customHeight="1"/>
     <row r="18" ht="16.5" customHeight="1"/>
     <row r="19" ht="16.5" customHeight="1"/>
@@ -4501,7 +4595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -5698,7 +5792,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5716,18 +5810,20 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -5735,18 +5831,20 @@
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1">
       <c r="A2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>72</v>
+      <c r="C2" s="5">
+        <v>2</v>
       </c>
       <c r="D2" s="5">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -5754,18 +5852,20 @@
     </row>
     <row r="3" spans="1:9" ht="16.5" customHeight="1">
       <c r="A3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>68</v>
+      <c r="C3" s="5">
+        <v>3</v>
       </c>
       <c r="D3" s="5">
-        <v>4</v>
-      </c>
-      <c r="E3" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -5773,18 +5873,20 @@
     </row>
     <row r="4" spans="1:9" ht="16.5" customHeight="1">
       <c r="A4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>69</v>
+      <c r="C4" s="5">
+        <v>0</v>
       </c>
       <c r="D4" s="5">
         <v>3</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -5792,18 +5894,20 @@
     </row>
     <row r="5" spans="1:9" ht="16.5" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>73</v>
+        <v>65</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="5">
+        <v>3</v>
+      </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>

</xml_diff>

<commit_message>
[Fix] LoadingScene Fix, SkillExplainUI
</commit_message>
<xml_diff>
--- a/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
+++ b/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="1650" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="6840" yWindow="1650" windowWidth="21600" windowHeight="11385" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="88">
   <si>
     <t>job</t>
   </si>
@@ -446,10 +446,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>일섬</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>은신</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -491,6 +487,34 @@
   </si>
   <si>
     <t>coolTime</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>출혈</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>출혈 스킬에 공격당할 시 지속데미지를 받는다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>castingTime</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>암살</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>durationTime</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>trueDamage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>animTime</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -845,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -2020,10 +2044,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1000"/>
+  <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2038,7 +2062,7 @@
     <col min="28" max="1026" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" customHeight="1">
+    <row r="1" spans="1:10" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2052,19 +2076,25 @@
         <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>79</v>
+      <c r="I1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.5" customHeight="1">
+    <row r="2" spans="1:10" ht="16.5" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -2089,8 +2119,14 @@
       <c r="H2">
         <v>1</v>
       </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>100</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="16.5" customHeight="1">
+    <row r="3" spans="1:10" ht="16.5" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -2115,8 +2151,14 @@
       <c r="H3">
         <v>1</v>
       </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>100</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1">
+    <row r="4" spans="1:10" ht="16.5" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2141,8 +2183,14 @@
       <c r="H4">
         <v>1</v>
       </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>100</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" ht="16.5" customHeight="1">
+    <row r="5" spans="1:10" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
@@ -2167,8 +2215,14 @@
       <c r="H5">
         <v>1</v>
       </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>100</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" ht="16.5" customHeight="1">
+    <row r="6" spans="1:10" ht="16.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -2193,8 +2247,14 @@
       <c r="H6">
         <v>1</v>
       </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>100</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" ht="16.5" customHeight="1">
+    <row r="7" spans="1:10" ht="16.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>54</v>
       </c>
@@ -2219,13 +2279,19 @@
       <c r="H7">
         <v>1</v>
       </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>100</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" ht="16.5" customHeight="1">
+    <row r="8" spans="1:10" ht="16.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>47</v>
@@ -2234,10 +2300,10 @@
         <v>3</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F8" s="7">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -2245,25 +2311,31 @@
       <c r="H8">
         <v>1</v>
       </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>100</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" ht="16.5" customHeight="1">
+    <row r="9" spans="1:10" ht="16.5" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9" s="4">
         <v>3</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F9" s="7">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>3</v>
@@ -2271,13 +2343,19 @@
       <c r="H9">
         <v>1</v>
       </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>100</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" ht="16.5" customHeight="1">
+    <row r="10" spans="1:10" ht="16.5" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>47</v>
@@ -2297,13 +2375,19 @@
       <c r="H10">
         <v>1</v>
       </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>100</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" ht="16.5" customHeight="1"/>
-    <row r="12" spans="1:8" ht="16.5" customHeight="1"/>
-    <row r="13" spans="1:8" ht="16.5" customHeight="1"/>
-    <row r="14" spans="1:8" ht="16.5" customHeight="1"/>
-    <row r="15" spans="1:8" ht="16.5" customHeight="1"/>
-    <row r="16" spans="1:8" ht="16.5" customHeight="1"/>
+    <row r="11" spans="1:10" ht="16.5" customHeight="1"/>
+    <row r="12" spans="1:10" ht="16.5" customHeight="1"/>
+    <row r="13" spans="1:10" ht="16.5" customHeight="1"/>
+    <row r="14" spans="1:10" ht="16.5" customHeight="1"/>
+    <row r="15" spans="1:10" ht="16.5" customHeight="1"/>
+    <row r="16" spans="1:10" ht="16.5" customHeight="1"/>
     <row r="17" ht="16.5" customHeight="1"/>
     <row r="18" ht="16.5" customHeight="1"/>
     <row r="19" ht="16.5" customHeight="1"/>
@@ -5831,7 +5915,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5840,7 +5924,8 @@
     <col min="2" max="2" width="35.21875" customWidth="1"/>
     <col min="3" max="3" width="9.77734375" customWidth="1"/>
     <col min="4" max="4" width="14.21875" customWidth="1"/>
-    <col min="5" max="6" width="9.77734375" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
     <col min="7" max="7" width="17.109375" customWidth="1"/>
     <col min="8" max="9" width="9.77734375" customWidth="1"/>
     <col min="10" max="26" width="8.21875" customWidth="1"/>
@@ -5849,22 +5934,26 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" customHeight="1">
       <c r="A1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="F1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
@@ -5884,8 +5973,12 @@
       <c r="E2" s="5">
         <v>0</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="F2" s="5">
+        <v>60</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
@@ -5905,8 +5998,12 @@
       <c r="E3" s="5">
         <v>0</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="F3" s="5">
+        <v>30</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
@@ -5926,8 +6023,12 @@
       <c r="E4" s="5">
         <v>0</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="F4" s="5">
+        <v>30</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
@@ -5947,19 +6048,37 @@
       <c r="E5" s="5">
         <v>3</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="5">
+        <v>30</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="A6" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>

</xml_diff>

<commit_message>
[Mod] Stat With Layer
</commit_message>
<xml_diff>
--- a/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
+++ b/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\HIGHFIVE\HIGHFIVE\Assets\Resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity_Project\TeamProject\Sparta06_TeamProject_HIGHFIVE\HIGHFIVE\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820AEC14-F162-46B8-99DD-01EDD50966B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="1650" windowWidth="21600" windowHeight="11385" tabRatio="500"/>
+    <workbookView xWindow="3015" yWindow="1770" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="85">
   <si>
     <t>job</t>
   </si>
@@ -201,15 +202,6 @@
     <t>나무</t>
   </si>
   <si>
-    <t>EL4</t>
-  </si>
-  <si>
-    <t>EP1</t>
-  </si>
-  <si>
-    <t>EP2</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -366,66 +358,62 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>블루</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>레드</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마법사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마법사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>도적</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>도적</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>도적</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>패자의 분노</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>레드</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>블루</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>배틀 페이즈에서 패배했을 시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>레드 몬스터 처치 시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>블루 몬스터 처치 시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>에픽</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>블루</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>레드</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>마법사</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>마법사</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>도적</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>도적</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>도적</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>패자의 분노</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>레드</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>블루</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>배틀 페이즈에서 패배했을 시</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>레드 몬스터 처치 시</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>블루 몬스터 처치 시</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>에픽</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>에픽 몬스터 처치 시</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -515,13 +503,17 @@
   </si>
   <si>
     <t>animTime</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>엘리트</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -866,10 +858,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -2043,7 +2035,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2076,22 +2068,22 @@
         <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1">
@@ -2166,7 +2158,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D4" s="4">
         <v>3</v>
@@ -2192,13 +2184,13 @@
     </row>
     <row r="5" spans="1:10" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -2224,13 +2216,13 @@
     </row>
     <row r="6" spans="1:10" ht="16.5" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D6" s="4">
         <v>3</v>
@@ -2256,13 +2248,13 @@
     </row>
     <row r="7" spans="1:10" ht="16.5" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D7" s="4">
         <v>3</v>
@@ -2288,13 +2280,13 @@
     </row>
     <row r="8" spans="1:10" ht="16.5" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D8" s="4">
         <v>3</v>
@@ -2320,13 +2312,13 @@
     </row>
     <row r="9" spans="1:10" ht="16.5" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D9" s="4">
         <v>3</v>
@@ -2352,13 +2344,13 @@
     </row>
     <row r="10" spans="1:10" ht="16.5" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D10" s="4">
         <v>3</v>
@@ -3380,11 +3372,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3426,7 +3418,7 @@
         <v>26</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1">
@@ -3463,7 +3455,7 @@
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3" s="5">
         <v>12</v>
@@ -3495,7 +3487,7 @@
     </row>
     <row r="4" spans="1:10" ht="16.5" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B4" s="5">
         <v>13</v>
@@ -3527,7 +3519,7 @@
     </row>
     <row r="5" spans="1:10" ht="16.5" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B5" s="5">
         <v>13</v>
@@ -3559,7 +3551,7 @@
     </row>
     <row r="6" spans="1:10" ht="16.5" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B6" s="5">
         <v>13</v>
@@ -3591,7 +3583,7 @@
     </row>
     <row r="7" spans="1:10" ht="16.5" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="B7" s="5">
         <v>15</v>
@@ -3622,100 +3614,37 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="5">
-        <v>10</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1</v>
-      </c>
-      <c r="E8" s="5">
-        <v>2</v>
-      </c>
-      <c r="F8" s="5">
-        <v>3</v>
-      </c>
-      <c r="G8" s="5">
-        <v>50</v>
-      </c>
-      <c r="H8" s="5">
-        <v>50</v>
-      </c>
-      <c r="I8" s="3">
-        <v>10</v>
-      </c>
-      <c r="J8" s="5">
-        <v>3</v>
-      </c>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="5">
-        <v>10</v>
-      </c>
-      <c r="C9" s="5">
-        <v>0</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1</v>
-      </c>
-      <c r="E9" s="5">
-        <v>2</v>
-      </c>
-      <c r="F9" s="5">
-        <v>3</v>
-      </c>
-      <c r="G9" s="5">
-        <v>50</v>
-      </c>
-      <c r="H9" s="5">
-        <v>50</v>
-      </c>
-      <c r="I9" s="3">
-        <v>30</v>
-      </c>
-      <c r="J9" s="5">
-        <v>3</v>
-      </c>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="5">
-        <v>10</v>
-      </c>
-      <c r="C10" s="5">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1</v>
-      </c>
-      <c r="E10" s="5">
-        <v>2</v>
-      </c>
-      <c r="F10" s="5">
-        <v>3</v>
-      </c>
-      <c r="G10" s="5">
-        <v>50</v>
-      </c>
-      <c r="H10" s="5">
-        <v>50</v>
-      </c>
-      <c r="I10" s="3">
-        <v>30</v>
-      </c>
-      <c r="J10" s="5">
-        <v>3</v>
-      </c>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="16.5" customHeight="1"/>
     <row r="12" spans="1:10" ht="16.5" customHeight="1"/>
@@ -4715,7 +4644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4737,31 +4666,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1">
@@ -4769,13 +4698,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E2" s="5">
         <v>100</v>
@@ -4798,13 +4727,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E3" s="5">
         <v>100</v>
@@ -4827,13 +4756,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E4" s="5">
         <v>100</v>
@@ -4856,13 +4785,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E5" s="5">
         <v>100</v>
@@ -4885,13 +4814,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E6" s="5">
         <v>100</v>
@@ -5911,7 +5840,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5934,35 +5863,35 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C2" s="5">
         <v>2</v>
@@ -5984,10 +5913,10 @@
     </row>
     <row r="3" spans="1:9" ht="16.5" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C3" s="5">
         <v>3</v>
@@ -6009,10 +5938,10 @@
     </row>
     <row r="4" spans="1:9" ht="16.5" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C4" s="5">
         <v>0</v>
@@ -6034,10 +5963,10 @@
     </row>
     <row r="5" spans="1:9" ht="16.5" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
@@ -6059,10 +5988,10 @@
     </row>
     <row r="6" spans="1:9" ht="16.5" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
[Update] Monster Buff Update
</commit_message>
<xml_diff>
--- a/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
+++ b/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity_Project\TeamProject\Sparta06_TeamProject_HIGHFIVE\HIGHFIVE\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C216F718-3A94-4490-B68C-B94B4182AD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BF76AC-0A82-4E3D-94BE-F5BEF3D711F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32925" yWindow="1275" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29775" yWindow="2325" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="88">
   <si>
     <t>job</t>
   </si>
@@ -380,14 +380,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>에픽</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>에픽 몬스터 처치 시</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>파이어볼</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -529,6 +521,10 @@
   </si>
   <si>
     <t>isSustain</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>엘리트 몬스터 처치 시</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -922,7 +918,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -2102,22 +2098,22 @@
         <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K1" s="1"/>
     </row>
@@ -2126,10 +2122,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
@@ -2158,7 +2154,7 @@
         <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>39</v>
@@ -2190,7 +2186,7 @@
         <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>39</v>
@@ -2219,10 +2215,10 @@
     </row>
     <row r="5" spans="1:11" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>39</v>
@@ -2251,10 +2247,10 @@
     </row>
     <row r="6" spans="1:11" ht="16.5" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>39</v>
@@ -3280,7 +3276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -3328,7 +3324,7 @@
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2" s="5">
         <v>10</v>
@@ -3360,7 +3356,7 @@
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" s="5">
         <v>15</v>
@@ -3488,7 +3484,7 @@
     </row>
     <row r="7" spans="1:10" ht="16.5" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B7" s="5">
         <v>100</v>
@@ -5748,8 +5744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5769,34 +5765,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1">
       <c r="A1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>58</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1">
@@ -5897,10 +5893,10 @@
     </row>
     <row r="5" spans="1:10" ht="16.5" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="C5" s="5">
         <v>5</v>
@@ -5929,10 +5925,10 @@
     </row>
     <row r="6" spans="1:10" ht="16.5" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C6" s="5">
         <v>0</v>
@@ -5961,10 +5957,10 @@
     </row>
     <row r="7" spans="1:10" ht="16.5" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="5">
         <v>0</v>
@@ -5993,10 +5989,10 @@
     </row>
     <row r="8" spans="1:10" ht="16.5" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" s="5">
         <v>0</v>
@@ -7037,15 +7033,15 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>3</v>
@@ -7175,7 +7171,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="B14" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:8">

</xml_diff>

<commit_message>
[Mod] Excel Monster ExpData
</commit_message>
<xml_diff>
--- a/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
+++ b/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29775" yWindow="2325" windowWidth="21600" windowHeight="11385" tabRatio="500"/>
+    <workbookView xWindow="29775" yWindow="2325" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -896,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3291,8 +3291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3363,7 +3363,7 @@
         <v>50</v>
       </c>
       <c r="I2" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J2" s="5">
         <v>3</v>
@@ -3392,10 +3392,10 @@
         <v>80</v>
       </c>
       <c r="H3" s="5">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="I3" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J3" s="5">
         <v>3</v>
@@ -3424,10 +3424,10 @@
         <v>100</v>
       </c>
       <c r="H4" s="5">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="I4" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J4" s="5">
         <v>3</v>
@@ -3453,13 +3453,13 @@
         <v>3</v>
       </c>
       <c r="G5" s="5">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="H5" s="5">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="I5" s="3">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="J5" s="5">
         <v>4</v>
@@ -3485,13 +3485,13 @@
         <v>3</v>
       </c>
       <c r="G6" s="5">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="H6" s="5">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="I6" s="3">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="J6" s="5">
         <v>4</v>
@@ -3502,7 +3502,7 @@
         <v>66</v>
       </c>
       <c r="B7" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C7" s="5">
         <v>15</v>
@@ -3517,13 +3517,13 @@
         <v>3</v>
       </c>
       <c r="G7" s="5">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="H7" s="5">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="I7" s="3">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J7" s="5">
         <v>4</v>
@@ -7062,7 +7062,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -7121,7 +7121,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="8">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H3" s="8">
         <v>300</v>

</xml_diff>

<commit_message>
[Mod] Rogue, HealKit Sprite or Animation add
</commit_message>
<xml_diff>
--- a/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
+++ b/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29775" yWindow="2325" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="29775" yWindow="2325" windowWidth="21600" windowHeight="11385" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -896,7 +896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -3291,7 +3291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -4564,7 +4564,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
[Mod] Mage Damage Fix
</commit_message>
<xml_diff>
--- a/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
+++ b/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity_Project\TeamProject\Sparta06_TeamProject_HIGHFIVE\HIGHFIVE\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226DB125-39CE-4BFF-8404-2652D13B40B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA4AC36-D238-4A9B-AAA1-0C3E5EC2C19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35190" yWindow="1605" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35190" yWindow="1605" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -2078,8 +2078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K994"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2175,10 +2175,10 @@
         <v>5</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F3" s="7">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -3288,7 +3288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[Fix] Elite Collider & AttackRange Fix / Exp Balance Fix
</commit_message>
<xml_diff>
--- a/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
+++ b/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity_Project\TeamProject\Sparta06_TeamProject_HIGHFIVE\HIGHFIVE\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9A81F8-9DE9-47DD-BB87-77BFE955F657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5637997B-2460-4CBC-A6A7-0D90DC32FF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35190" yWindow="1605" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4591,7 +4591,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4662,7 +4662,7 @@
         <v>50</v>
       </c>
       <c r="I2" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J2" s="5">
         <v>3</v>
@@ -4694,7 +4694,7 @@
         <v>80</v>
       </c>
       <c r="I3" s="3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J3" s="5">
         <v>3</v>
@@ -4726,7 +4726,7 @@
         <v>100</v>
       </c>
       <c r="I4" s="3">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J4" s="5">
         <v>3</v>
@@ -4822,7 +4822,7 @@
         <v>600</v>
       </c>
       <c r="I7" s="3">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="J7" s="5">
         <v>4</v>

</xml_diff>

<commit_message>
[Fix] Warrior, Rogue atkRange
전사, 도적 공격 범위 수정
</commit_message>
<xml_diff>
--- a/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
+++ b/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity_Project\TeamProject\Sparta06_TeamProject_HIGHFIVE\HIGHFIVE\Assets\Resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\HIGHFIVE\HIGHFIVE\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5637997B-2460-4CBC-A6A7-0D90DC32FF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35190" yWindow="1605" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35190" yWindow="1605" windowWidth="21600" windowHeight="11385" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <sheet name="Items" sheetId="4" r:id="rId5"/>
     <sheet name="Sheet2" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -535,7 +534,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -890,11 +889,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -968,7 +967,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -1006,7 +1005,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F3" s="1">
         <v>1.3</v>
@@ -2075,7 +2074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K994"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
@@ -3285,7 +3284,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
@@ -4587,11 +4586,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5859,7 +5858,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7055,7 +7054,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
[Mod] Rougue Q Skill range
1 => 1.5
</commit_message>
<xml_diff>
--- a/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
+++ b/HIGHFIVE/Assets/Resources/Data/HIGHFIVE_Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\HIGHFIVE\HIGHFIVE\Assets\Resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rgh99\OneDrive\문서\GitHub\HIGHFIVE\HIGHFIVE\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5A6D05-D53F-4A1A-B845-DBA8C3E0AB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31515" yWindow="1845" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="6450" yWindow="1335" windowWidth="19845" windowHeight="13470" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <sheet name="Items" sheetId="4" r:id="rId5"/>
     <sheet name="Sheet2" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -534,7 +535,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -889,7 +890,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2074,11 +2075,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K994"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2203,7 +2204,7 @@
         <v>39</v>
       </c>
       <c r="D4" s="4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -3284,7 +3285,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
@@ -4586,7 +4587,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5858,7 +5859,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7054,7 +7055,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>